<commit_message>
TST: Update tests for changes to Area and Problem
</commit_message>
<xml_diff>
--- a/tests/example.xlsx
+++ b/tests/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14320" tabRatio="500"/>
+    <workbookView xWindow="7920" yWindow="360" windowWidth="25600" windowHeight="14320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Area" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -106,6 +106,63 @@
   </si>
   <si>
     <t>Boulder</t>
+  </si>
+  <si>
+    <t>Problem 7</t>
+  </si>
+  <si>
+    <t>Problem 8</t>
+  </si>
+  <si>
+    <t>Problem 9</t>
+  </si>
+  <si>
+    <t>Problem 10</t>
+  </si>
+  <si>
+    <t>Problem 11</t>
+  </si>
+  <si>
+    <t>Problem 12</t>
+  </si>
+  <si>
+    <t>Problem 13</t>
+  </si>
+  <si>
+    <t>Problem 14</t>
+  </si>
+  <si>
+    <t>Problem 15</t>
+  </si>
+  <si>
+    <t>Problem 16</t>
+  </si>
+  <si>
+    <t>Problem 17</t>
+  </si>
+  <si>
+    <t>Problem 18</t>
+  </si>
+  <si>
+    <t>Problem 19</t>
+  </si>
+  <si>
+    <t>Problem 20</t>
+  </si>
+  <si>
+    <t>Problem 21</t>
+  </si>
+  <si>
+    <t>Problem 22</t>
+  </si>
+  <si>
+    <t>Problem 23</t>
+  </si>
+  <si>
+    <t>Problem 24</t>
+  </si>
+  <si>
+    <t>Problem 25</t>
   </si>
 </sst>
 </file>
@@ -243,8 +300,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -309,7 +370,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -331,6 +392,8 @@
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -352,6 +415,8 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -681,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -820,10 +885,10 @@
         <v>13</v>
       </c>
       <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
         <v>1</v>
-      </c>
-      <c r="D29">
-        <v>5</v>
       </c>
       <c r="E29" t="s">
         <v>16</v>
@@ -840,7 +905,7 @@
         <v>2</v>
       </c>
       <c r="D30">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E30" t="s">
         <v>17</v>
@@ -851,10 +916,10 @@
         <v>21</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C31">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D31">
         <v>3</v>
@@ -868,10 +933,10 @@
         <v>22</v>
       </c>
       <c r="B32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C32">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D32">
         <v>2</v>
@@ -885,10 +950,10 @@
         <v>23</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C33">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -902,15 +967,338 @@
         <v>24</v>
       </c>
       <c r="B34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>3</v>
+      </c>
+      <c r="E35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36">
+        <v>6</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37">
+        <v>6</v>
+      </c>
+      <c r="D37">
+        <v>5</v>
+      </c>
+      <c r="E37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38">
+        <v>7</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39">
+        <v>8</v>
+      </c>
+      <c r="D39">
+        <v>3</v>
+      </c>
+      <c r="E39" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40">
+        <v>11</v>
+      </c>
+      <c r="D40">
+        <v>3</v>
+      </c>
+      <c r="E40" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>35</v>
+      </c>
+      <c r="B41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>36</v>
+      </c>
+      <c r="B42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42">
+        <v>13</v>
+      </c>
+      <c r="D42">
+        <v>3</v>
+      </c>
+      <c r="E42" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>37</v>
+      </c>
+      <c r="B43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43">
+        <v>5</v>
+      </c>
+      <c r="D43">
+        <v>4</v>
+      </c>
+      <c r="E43" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44">
+        <v>6</v>
+      </c>
+      <c r="D44">
+        <v>5</v>
+      </c>
+      <c r="E44" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>39</v>
+      </c>
+      <c r="B45" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45">
+        <v>7</v>
+      </c>
+      <c r="D45">
+        <v>4</v>
+      </c>
+      <c r="E45" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>4</v>
+      </c>
+      <c r="E46" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47">
+        <v>9</v>
+      </c>
+      <c r="D47">
+        <v>3</v>
+      </c>
+      <c r="E47" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48" t="s">
         <v>15</v>
       </c>
-      <c r="C34">
+      <c r="C48">
+        <v>7</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>43</v>
+      </c>
+      <c r="B49" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49">
+        <v>7</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="E49" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>44</v>
+      </c>
+      <c r="B50" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50">
+        <v>4</v>
+      </c>
+      <c r="D50">
+        <v>3</v>
+      </c>
+      <c r="E50" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" t="s">
+        <v>15</v>
+      </c>
+      <c r="C51">
         <v>6</v>
       </c>
-      <c r="D34">
+      <c r="D51">
+        <v>3</v>
+      </c>
+      <c r="E51" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>46</v>
+      </c>
+      <c r="B52" t="s">
+        <v>15</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
+      </c>
+      <c r="D52">
+        <v>4</v>
+      </c>
+      <c r="E52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>47</v>
+      </c>
+      <c r="B53" t="s">
+        <v>15</v>
+      </c>
+      <c r="C53">
+        <v>6</v>
+      </c>
+      <c r="D53">
         <v>5</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E53" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>